<commit_message>
Use Case is updated
</commit_message>
<xml_diff>
--- a/Documents/Use Case Diagram/usecase_v1.xlsx
+++ b/Documents/Use Case Diagram/usecase_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ossarioglu/SWE_Coding/SWE574/SWE574-SWEet_Dewarriors/Documents/Use Case Diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB642BE4-00FF-FD40-AC04-10510CC03EBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FA9814-6B95-654D-A812-00EFEB56E72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30900" yWindow="10160" windowWidth="28100" windowHeight="21260" xr2:uid="{F772AB01-D0BE-3243-B730-C926DEE3E4AA}"/>
   </bookViews>
@@ -144,14 +144,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="tr-TR" sz="1800">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>System</a:t>
-          </a:r>
+          <a:endParaRPr lang="tr-TR" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3018,6 +3015,510 @@
         </a:prstGeom>
         <a:ln w="12700">
           <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571046</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>87932</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="57" name="Grup 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C6DE015E-17AA-B546-809D-DF137D186737}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="11176000" y="2667000"/>
+          <a:ext cx="952046" cy="1688132"/>
+          <a:chOff x="2588762" y="2095500"/>
+          <a:chExt cx="952046" cy="1688132"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="58" name="Oval 57">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9528F01-256A-4847-833F-6D4E5500C823}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2755900" y="2095500"/>
+            <a:ext cx="304800" cy="317500"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="tr-TR" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="60" name="Düz Bağlayıcı 59">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D08298C-9381-7C46-8A26-8BFAA7FDEAF5}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr>
+            <a:stCxn id="58" idx="4"/>
+          </xdr:cNvCxnSpPr>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2908300" y="2413000"/>
+            <a:ext cx="0" cy="635000"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="62" name="Düz Bağlayıcı 61">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F55912B9-0158-3F4C-8C86-C7179E7CB2CC}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm flipH="1">
+            <a:off x="2643847" y="3049516"/>
+            <a:ext cx="266700" cy="355600"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="64" name="Düz Bağlayıcı 63">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C2DFEC5-AB3F-2E4B-A671-2E2B4E6E7F23}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2911226" y="3055578"/>
+            <a:ext cx="265176" cy="355600"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:cxnSp macro="">
+        <xdr:nvCxnSpPr>
+          <xdr:cNvPr id="66" name="Düz Bağlayıcı 65">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D152B60-E960-9A4F-AB00-0CE411541045}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvCxnSpPr/>
+        </xdr:nvCxnSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="16200000">
+            <a:off x="2907516" y="2326452"/>
+            <a:ext cx="0" cy="637508"/>
+          </a:xfrm>
+          <a:prstGeom prst="line">
+            <a:avLst/>
+          </a:prstGeom>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+      </xdr:cxnSp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="67" name="Metin kutusu 66">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DCFBA90-7CFB-EC42-AF00-2AECECB93BE6}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="2603500" y="3378200"/>
+            <a:ext cx="937308" cy="405432"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="tx1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+            <a:spAutoFit/>
+          </a:bodyPr>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="tr-TR" sz="2000"/>
+              <a:t>System</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="69" name="Oval 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13626498-7121-BC45-9999-4314305E2899}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8928100" y="2832100"/>
+          <a:ext cx="1346200" cy="660400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1200"/>
+            <a:t>Notification</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="70" name="Oval 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54DFD308-2E21-B742-97EB-BE5980A744E7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8953500" y="3721100"/>
+          <a:ext cx="1346200" cy="660400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1200"/>
+            <a:t>Activity Stream Info</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Düz Ok Bağlayıcısı 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70C9D94A-EE10-284B-B9D5-B3CEC5960F76}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="69" idx="6"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10274300" y="3162300"/>
+          <a:ext cx="990600" cy="241300"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="72" name="Düz Ok Bağlayıcısı 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BA00A54-9B00-464C-95FC-5EE329E0000F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10312400" y="3556000"/>
+          <a:ext cx="1104900" cy="393700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
           <a:tailEnd type="triangle"/>
         </a:ln>
       </xdr:spPr>

</xml_diff>

<commit_message>
use case diagram is updated
</commit_message>
<xml_diff>
--- a/Documents/Use Case Diagram/usecase_v1.xlsx
+++ b/Documents/Use Case Diagram/usecase_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ossarioglu/SWE_Coding/SWE574/SWE574-SWEet_Dewarriors/Documents/Use Case Diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FA9814-6B95-654D-A812-00EFEB56E72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9AA15E-2C1F-484C-A19A-75EE5A0C20E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30900" yWindow="10160" windowWidth="28100" windowHeight="21260" xr2:uid="{F772AB01-D0BE-3243-B730-C926DEE3E4AA}"/>
   </bookViews>
@@ -1258,8 +1258,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2588762" y="2095500"/>
-          <a:ext cx="681267" cy="1688132"/>
+          <a:off x="2586288" y="2042721"/>
+          <a:ext cx="681267" cy="1645908"/>
           <a:chOff x="2588762" y="2095500"/>
           <a:chExt cx="681267" cy="1688132"/>
         </a:xfrm>
@@ -1528,8 +1528,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="2512562" y="5549900"/>
-          <a:ext cx="881065" cy="1688132"/>
+          <a:off x="2510088" y="5407396"/>
+          <a:ext cx="880240" cy="1645909"/>
           <a:chOff x="2588762" y="2095500"/>
           <a:chExt cx="881065" cy="1688132"/>
         </a:xfrm>
@@ -3061,8 +3061,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="11176000" y="2667000"/>
-          <a:ext cx="952046" cy="1688132"/>
+          <a:off x="11165279" y="2598387"/>
+          <a:ext cx="951222" cy="1645909"/>
           <a:chOff x="2588762" y="2095500"/>
           <a:chExt cx="952046" cy="1688132"/>
         </a:xfrm>
@@ -3521,6 +3521,618 @@
         <a:ln w="12700">
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Oval 73">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20546CA-E808-0D4E-BC98-3FF970CCC6B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9144000" y="4622800"/>
+          <a:ext cx="1866900" cy="660400"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1200"/>
+            <a:t>Recommendation</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="75" name="Düz Ok Bağlayıcısı 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE727E49-E893-A940-900D-E0A73110D67C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10312400" y="3797300"/>
+          <a:ext cx="1028700" cy="812800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="79" name="Düz Ok Bağlayıcısı 78">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB369591-77FC-AB41-AB17-785E7031492B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6108700" y="5080000"/>
+          <a:ext cx="3060700" cy="647700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="81" name="Düz Ok Bağlayıcısı 80">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8362AC92-8BDF-1F4F-AF6E-234DE184FBFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7226300" y="4495800"/>
+          <a:ext cx="2108200" cy="1117600"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>251028</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160213</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="83" name="Düz Ok Bağlayıcısı 82">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1116A484-5694-CC4D-ADAA-3D09DC50BA02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="9" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="7797800" y="3378200"/>
+          <a:ext cx="1533728" cy="2268413"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="84" name="Düz Ok Bağlayıcısı 83">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{49313F0A-E935-8A44-952B-761C0C7BD75D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6070600" y="2336800"/>
+          <a:ext cx="3060700" cy="2425700"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:prstDash val="dash"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="85" name="Metin kutusu 84">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F548935-81E1-BA45-89D8-4CC25E6E92EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1765300" y="88900"/>
+          <a:ext cx="1257300" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="tr-TR" sz="1600"/>
+            <a:t>uC Sharity</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>101600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="93" name="Dikdörtgen 92">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEBBD81C-A960-7642-8C72-B58F6829349D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1752600" y="76200"/>
+          <a:ext cx="10668000" cy="9232900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="tr-TR" sz="1800">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>429762</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="94" name="Düz Bağlayıcı 93">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB7DBA62-3304-1244-9046-52B7130DC190}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="2906262" y="88900"/>
+          <a:ext cx="2038" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>86862</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>259773</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57727</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="96" name="Düz Bağlayıcı 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96BB3CEE-13E7-4B4C-9386-5B4CF22CA4ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1737862" y="454891"/>
+          <a:ext cx="998411" cy="6927"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>265545</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>103910</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>427182</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57727</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="Düz Bağlayıcı 98">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{041AC1EA-1700-D34D-88CA-C128B187BBC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="2742045" y="305955"/>
+          <a:ext cx="161637" cy="155863"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -3841,7 +4453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5E8FAF-D5A7-534E-AF9E-4FF772F82925}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="77" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>